<commit_message>
Graph for realtive success rate by email source.
</commit_message>
<xml_diff>
--- a/Stats/Data/echoTreePerf.xlsx
+++ b/Stats/Data/echoTreePerf.xlsx
@@ -17,9 +17,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>SubjID</t>
-  </si>
   <si>
     <t>DBId</t>
   </si>
@@ -46,6 +43,9 @@
   </si>
   <si>
     <t>Depth_2</t>
+  </si>
+  <si>
+    <t>EmailSrc</t>
   </si>
 </sst>
 </file>
@@ -387,41 +387,41 @@
   <dimension ref="A1:J573"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A183" sqref="A183:J573"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Corrected bar graph to have proper shading and scale.
</commit_message>
<xml_diff>
--- a/Stats/Data/echoTreePerf.xlsx
+++ b/Stats/Data/echoTreePerf.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>DBId</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>EmailSrc</t>
+  </si>
+  <si>
+    <t>Mean success Henry:</t>
+  </si>
+  <si>
+    <t>Mean success EmpX</t>
   </si>
 </sst>
 </file>
@@ -384,15 +390,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J573"/>
+  <dimension ref="A1:L573"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -424,7 +434,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -455,8 +465,15 @@
       <c r="J2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <f>AVERAGE(H2:H182)</f>
+        <v>4.7087292817679556</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -487,8 +504,15 @@
       <c r="J3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3">
+        <f>AVERAGE(H183:H573)</f>
+        <v>15.213069053708445</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -520,7 +544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -552,7 +576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -584,7 +608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -616,7 +640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -648,7 +672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -680,7 +704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -712,7 +736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -744,7 +768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -776,7 +800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -808,7 +832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -840,7 +864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -872,7 +896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>

</xml_diff>